<commit_message>
1.5 Removed many unused code and elements that where not needed
</commit_message>
<xml_diff>
--- a/price_list.xlsx
+++ b/price_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pscharnetzki\PycharmProjects\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F5310D-2DC9-438C-9625-F54822218438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6C233D-C868-4182-B8E8-B9939745B207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{040EAB17-3D51-4BCE-933F-213A1E0AC919}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{040EAB17-3D51-4BCE-933F-213A1E0AC919}"/>
   </bookViews>
   <sheets>
     <sheet name="40495396" sheetId="3" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="69">
   <si>
     <t>Summe</t>
   </si>
@@ -273,6 +273,47 @@
   </si>
   <si>
     <t xml:space="preserve"> Dell Mobile Precision Workstation 5680 CTO, 4 Jahre Pro Support mit NFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14" 2 in 1 Notebook mit Tabletfunktion für ein flexibles Arbeiten im Büro und beim mobilen Arbeiten. (deutsches Tastaturlayout)
+Technische Daten
+Prozessor
+Intel® Core™ i5-1245U der 12. Generation (12 MB Cache, 10 Cores, bis zu 4,40 GHz Turbo, vPro® Enterprise)
+Grafikkarte
+Intel® Iris® XE Grafikkarte für i5-1245U Prozessoren mit vPro und 16 GB DDR4-Arbeitsspeicher für Laptops
+Bildschirm
+Laptop mit 14"-FHD-Display (1.920 x 1.080), AG, ohne Touchfunktion, weiter Betrachtungswinkel, 250 cd/m², FHD-IR-Kamera + IP, WLAN, WWAN, Carbonfaser
+Arbeitsspeicher 
+16 GB DDR4-Arbeitsspeicher, 3.200 MHz, Non-ECC, integriert
+Festplatte
+256-GB-M.2-PCIe-NVMe-SSD – Klasse 35
+Support-Services
+kein Service-Upgrade, 36 Monat(e)
+Tastatur
+Tastatur mit Hintergrundbeleuchtung und 80 Tasten – Deutsch
+Anschlüsse
+2 USB Typ-C® Thunderbolt™ 4.0-Anschlüsse mit Power Delivery und DisplayPort 1.4
+1 USB 3.2 Gen 1-Anschluss mit PowerShare
+1 Headsetanschluss (Kopfhörer und Mikrofon)
+1 HDMI 2.0-Anschluss
+Steckplätze
+1 x Smartcard-Lesegerät (optional)
+1 microSIM-Kartensteckplatz (optional)
+Kamera
+2,7 mm, 720p bei 30 fps, HD-RGB-Webcam
+6 mm, 720p bei 30 fps, HD-RGB-Webcam
+3,25 mm, 1080p bei 30 fps, FHD-RGB+ IR-Webcam mit Erkennung von menschlicher Anwesenheit und ALS
+6 mm, 1.080p bei 30 fps FHD-RGB- + IR-Webcam mit Erkennung menschlicher Anwesenheit und ALS
+Audio und Lautsprecher
+Stereolautsprecher mit Waves MaxxAudio® Pro, 2 W x 2 = 4 W insgesamt
+2 Mikrofone mit Rauschunterdrückung
+Intelligent Audio mit neuronaler Rauschunterdrückung
+Wireless 
+Wireless-Karte für Intel® Wi-Fi 6E AX211, 2 x 2, 802.11ax, mit Bluetooth®
+Hauptakku
+ExpressCharge™-fähiger Akku mit 4 Zellen und 58 Wh
+Stromversorgung
+Typ-C-Adapter mit 65 W                                                                            </t>
   </si>
 </sst>
 </file>
@@ -1017,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67BFC60F-F20B-4DE4-9BED-CE868DF63EDD}">
   <dimension ref="A1:G113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,7 +1070,7 @@
     <col min="4" max="4" width="13" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="13" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="13" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="57" t="s">
         <v>65</v>
       </c>
@@ -1041,18 +1082,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="35"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="11"/>
       <c r="D3" s="12"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="55" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="45" t="s">
         <v>38</v>
       </c>
@@ -1064,7 +1108,7 @@
         <v>28.74</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="46" t="s">
         <v>30</v>
       </c>
@@ -1075,7 +1119,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
         <v>1</v>
       </c>
@@ -1086,7 +1130,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
         <v>31</v>
       </c>
@@ -1097,7 +1141,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>0</v>
       </c>
@@ -1111,11 +1155,11 @@
         <v>31.346875000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>5</v>
       </c>
@@ -1123,7 +1167,7 @@
       <c r="C10" s="11"/>
       <c r="D10" s="12"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="46" t="s">
         <v>39</v>
       </c>
@@ -1135,7 +1179,7 @@
         <v>28.74</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="46" t="s">
         <v>30</v>
       </c>
@@ -1146,7 +1190,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="46" t="s">
         <v>32</v>
       </c>
@@ -1157,7 +1201,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="46" t="s">
         <v>31</v>
       </c>
@@ -1168,7 +1212,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="47" t="s">
         <v>33</v>
       </c>
@@ -1179,7 +1223,7 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>0</v>
       </c>

</xml_diff>